<commit_message>
Added healing; Added animation events; Changed animation data; Added bullet time;
</commit_message>
<xml_diff>
--- a/DesignDocuments/机制、系统、数值/动画事件表.xlsx
+++ b/DesignDocuments/机制、系统、数值/动画事件表.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -28,99 +28,117 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>DelayInput</t>
+  </si>
+  <si>
+    <t>BlockInput</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttackEnd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttackStepDIstance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>事件意义</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缓存角色动作输入; 1 = true, 0 = false;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>屏蔽角色移动操作; 1 = true，0 = false;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>屏蔽角色动作操作; 1 = true，0 = false;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>标志攻击开始</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>标志攻击结束</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击位移速度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击位移距离</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>治疗一次角色</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Frozen</t>
-  </si>
-  <si>
-    <t>DelayInput</t>
-  </si>
-  <si>
-    <t>BlockInput</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>AttackBegin</t>
-  </si>
-  <si>
-    <t>AttackEnd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Regenerate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>AttackStepSpeed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AttackStepDIstance</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>N</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>N</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>float</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>float</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>N/A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>事件意义</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>缓存角色动作输入; 1 = true, 0 = false;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>屏蔽角色移动操作; 1 = true，0 = false;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>屏蔽角色动作操作; 1 = true，0 = false;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>标志攻击开始</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>标志攻击结束</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻击位移速度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻击位移距离</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -473,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -498,104 +516,118 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
       <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>